<commit_message>
Se adicionó la funcionalidad para mostrar el dataFrame de plazas-tarifas
</commit_message>
<xml_diff>
--- a/data/tarifas_GFM.xlsx
+++ b/data/tarifas_GFM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\gfm\Python-project-anunciantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\gfm\streamlit-demo\prod\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C25FA7E-194B-4AE2-957F-1355E60F47B3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD55705D-FD93-4260-9312-B2F6EFE286C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="38">
   <si>
     <t>PLAZA</t>
   </si>
@@ -137,82 +137,6 @@
   </si>
   <si>
     <t>MATAMOROS</t>
-  </si>
-  <si>
-    <t>REPITE TRANSMISION DE MENCIONES</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>6:00-9:00 AM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>9:00- 12:00 AM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>12:00- 15:00 PM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>15:00- 18:00 PM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>18:00- 21:00 PM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>21:00- 23:00 PM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>23:00- 1:00 AM</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">HECHOS NOCHE </t>
   </si>
   <si>
     <t>NACIONAL</t>
@@ -228,17 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,16 +175,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -280,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -314,57 +218,34 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -373,8 +254,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -687,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434E9FDD-879A-4363-B04D-C869C9708562}">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="B56" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +578,6 @@
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,278 +1482,197 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B54" s="10">
-        <v>6</v>
-      </c>
-      <c r="C54" s="10">
-        <v>14</v>
-      </c>
-      <c r="D54" s="11">
+      <c r="B54" s="9">
+        <v>6</v>
+      </c>
+      <c r="C54" s="9">
+        <v>14</v>
+      </c>
+      <c r="D54" s="10">
         <v>619.85</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="E54" s="3"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="10">
-        <v>14</v>
-      </c>
-      <c r="C55" s="10">
-        <v>18</v>
-      </c>
-      <c r="D55" s="11">
+      <c r="B55" s="9">
+        <v>14</v>
+      </c>
+      <c r="C55" s="9">
+        <v>18</v>
+      </c>
+      <c r="D55" s="10">
         <v>1151.1500000000001</v>
       </c>
       <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B56" s="10">
-        <v>18</v>
-      </c>
-      <c r="C56" s="10">
+      <c r="B56" s="9">
+        <v>18</v>
+      </c>
+      <c r="C56" s="9">
         <v>24</v>
       </c>
-      <c r="D56" s="11">
+      <c r="D56" s="10">
         <v>1771</v>
       </c>
       <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="9">
         <v>0</v>
       </c>
-      <c r="C57" s="10">
-        <v>6</v>
-      </c>
-      <c r="D57" s="11">
+      <c r="C57" s="9">
+        <v>6</v>
+      </c>
+      <c r="D57" s="10">
         <v>1771</v>
       </c>
       <c r="E57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B58" s="11">
-        <v>6</v>
-      </c>
-      <c r="C58" s="11">
+      <c r="B58" s="10">
+        <v>6</v>
+      </c>
+      <c r="C58" s="10">
         <v>9</v>
       </c>
-      <c r="D58" s="11">
+      <c r="D58" s="10">
         <v>25234.45</v>
       </c>
       <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B59" s="10">
         <v>9</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="10">
         <v>12</v>
       </c>
-      <c r="D59" s="11">
+      <c r="D59" s="10">
         <v>52713.7</v>
       </c>
       <c r="E59" s="3"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="11">
+      <c r="B60" s="10">
         <v>12</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="10">
         <v>15</v>
       </c>
-      <c r="D60" s="11">
+      <c r="D60" s="10">
         <v>43481.5</v>
       </c>
       <c r="E60" s="3"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="11">
+      <c r="B61" s="10">
         <v>15</v>
       </c>
-      <c r="C61" s="11">
-        <v>18</v>
-      </c>
-      <c r="D61" s="11">
+      <c r="C61" s="10">
+        <v>18</v>
+      </c>
+      <c r="D61" s="10">
         <v>65685.100000000006</v>
       </c>
       <c r="E61" s="3"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="11">
-        <v>18</v>
-      </c>
-      <c r="C62" s="11">
+      <c r="B62" s="10">
+        <v>18</v>
+      </c>
+      <c r="C62" s="10">
         <v>21</v>
       </c>
-      <c r="D62" s="11">
+      <c r="D62" s="10">
         <v>127015.2</v>
       </c>
       <c r="E62" s="3"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B63" s="11">
+      <c r="B63" s="10">
         <v>21</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="10">
         <v>23</v>
       </c>
-      <c r="D63" s="11">
+      <c r="D63" s="10">
         <v>119954.2</v>
       </c>
       <c r="E63" s="3"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="11">
+      <c r="B64" s="10">
         <v>23</v>
       </c>
-      <c r="C64" s="11">
+      <c r="C64" s="10">
         <v>1</v>
       </c>
-      <c r="D64" s="11">
+      <c r="D64" s="10">
         <v>53901.65</v>
       </c>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B65" s="11">
+      <c r="B65" s="10">
         <v>1</v>
       </c>
-      <c r="C65" s="11">
-        <v>6</v>
-      </c>
-      <c r="D65" s="11">
+      <c r="C65" s="10">
+        <v>6</v>
+      </c>
+      <c r="D65" s="10">
         <v>53901.65</v>
       </c>
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="11">
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="10">
         <v>144590</v>
       </c>
-      <c r="E66" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I68" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J68" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="K68" s="12">
-        <v>25234.45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I69" s="9"/>
-      <c r="J69" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="K69" s="12">
-        <v>52713.7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I70" s="9"/>
-      <c r="J70" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K70" s="12">
-        <v>43481.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I71" s="9"/>
-      <c r="J71" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="K71" s="12">
-        <v>65865.100000000006</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I72" s="9"/>
-      <c r="J72" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K72" s="12">
-        <v>127015.2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I73" s="9"/>
-      <c r="J73" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="K73" s="12">
-        <v>119954.2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I74" s="9"/>
-      <c r="J74" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K74" s="12">
-        <v>53901.65</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="I75" s="9"/>
-      <c r="J75" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="K75" s="12">
-        <v>144590</v>
-      </c>
+      <c r="E66" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I68:I75"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2016,25 +1814,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>46</v>
+      <c r="D1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1">
         <v>6</v>
@@ -2048,7 +1846,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1">
         <v>9</v>
@@ -2062,7 +1860,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -2076,7 +1874,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
@@ -2090,7 +1888,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -2104,7 +1902,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1">
         <v>21</v>
@@ -2118,7 +1916,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1">
         <v>23</v>
@@ -2132,7 +1930,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -2146,7 +1944,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B10" s="7">
         <v>1</v>
@@ -2160,7 +1958,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2168,7 +1966,7 @@
         <v>289181.3</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se adicionó la funcionalidad para mostrar el dataFrame de tarifas nacionales
</commit_message>
<xml_diff>
--- a/data/tarifas_GFM.xlsx
+++ b/data/tarifas_GFM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\gfm\streamlit-demo\prod\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD55705D-FD93-4260-9312-B2F6EFE286C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E53E0CC-94E9-4713-AEF8-193D814BDD1B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" activeTab="2" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
   </bookViews>
   <sheets>
     <sheet name="PLAZAS_TARIFAS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="36">
   <si>
     <t>PLAZA</t>
   </si>
@@ -140,12 +140,6 @@
   </si>
   <si>
     <t>NACIONAL</t>
-  </si>
-  <si>
-    <t>HECHOS DE NOCHE</t>
-  </si>
-  <si>
-    <t>ESPECIAL</t>
   </si>
 </sst>
 </file>
@@ -569,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434E9FDD-879A-4363-B04D-C869C9708562}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B56" workbookViewId="0">
+    <sheetView topLeftCell="B50" workbookViewId="0">
       <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
@@ -1802,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E191E4-A2D8-441B-8AD8-3523E2EF823B}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,9 +1820,7 @@
       <c r="D1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1964,9 +1956,6 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1">
         <v>289181.3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizando archivo de tarifas -- se agregó el CANAL de SANLUIS
</commit_message>
<xml_diff>
--- a/data/tarifas_GFM.xlsx
+++ b/data/tarifas_GFM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\gfm\streamlit-demo\prod\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E53E0CC-94E9-4713-AEF8-193D814BDD1B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F01E6F9-FA3B-49FA-BF20-096B42479876}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" activeTab="2" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
   <si>
     <t>PLAZA</t>
   </si>
@@ -561,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434E9FDD-879A-4363-B04D-C869C9708562}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="B50" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,6 +1666,74 @@
       </c>
       <c r="E66" s="3"/>
     </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="1">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1">
+        <v>14</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1377.7</v>
+      </c>
+      <c r="E67" s="1">
+        <v>7808.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68" s="1">
+        <v>14</v>
+      </c>
+      <c r="C68" s="1">
+        <v>18</v>
+      </c>
+      <c r="D68" s="1">
+        <v>2559.9</v>
+      </c>
+      <c r="E68" s="1">
+        <v>7808.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B69" s="1">
+        <v>18</v>
+      </c>
+      <c r="C69" s="1">
+        <v>24</v>
+      </c>
+      <c r="D69" s="1">
+        <v>3937.6</v>
+      </c>
+      <c r="E69" s="1">
+        <v>7808.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
+        <v>6</v>
+      </c>
+      <c r="D70" s="1">
+        <v>3937.6</v>
+      </c>
+      <c r="E70" s="1">
+        <v>7808.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1676,7 +1744,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,7 +1865,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se corrigió para guardar el archivo que se sube al directorio data ..
</commit_message>
<xml_diff>
--- a/data/tarifas_GFM.xlsx
+++ b/data/tarifas_GFM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\gfm\streamlit-demo\prod\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F01E6F9-FA3B-49FA-BF20-096B42479876}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3F3797-A597-4089-A8CE-B6E381B29460}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" activeTab="2" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" activeTab="1" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
   </bookViews>
   <sheets>
     <sheet name="PLAZAS_TARIFAS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="35">
   <si>
     <t>PLAZA</t>
   </si>
@@ -91,9 +91,6 @@
     <t>153-CIUDADJUAREZCANAL1</t>
   </si>
   <si>
-    <t>CIUDAD JUAREZ</t>
-  </si>
-  <si>
     <t>155-CHIHUAHUACANAL1</t>
   </si>
   <si>
@@ -133,13 +130,13 @@
     <t xml:space="preserve">TORREON </t>
   </si>
   <si>
-    <t xml:space="preserve">CD JUAREZ </t>
-  </si>
-  <si>
     <t>MATAMOROS</t>
   </si>
   <si>
     <t>NACIONAL</t>
+  </si>
+  <si>
+    <t>CIUDAD_JUAREZ</t>
   </si>
 </sst>
 </file>
@@ -563,13 +560,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434E9FDD-879A-4363-B04D-C869C9708562}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -865,7 +862,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
         <v>6</v>
@@ -882,7 +879,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>14</v>
@@ -899,7 +896,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>18</v>
@@ -916,7 +913,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -933,7 +930,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1">
         <v>6</v>
@@ -950,7 +947,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
         <v>14</v>
@@ -967,7 +964,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>18</v>
@@ -984,7 +981,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1001,7 +998,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1">
         <v>6</v>
@@ -1018,7 +1015,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>14</v>
@@ -1035,7 +1032,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
         <v>18</v>
@@ -1052,7 +1049,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1137,7 +1134,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1">
         <v>6</v>
@@ -1154,7 +1151,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1">
         <v>14</v>
@@ -1171,7 +1168,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1">
         <v>18</v>
@@ -1188,7 +1185,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -1273,7 +1270,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B42" s="1">
         <v>6</v>
@@ -1290,7 +1287,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="1">
         <v>14</v>
@@ -1307,7 +1304,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" s="1">
         <v>18</v>
@@ -1324,7 +1321,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -1341,7 +1338,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B46" s="1">
         <v>6</v>
@@ -1358,7 +1355,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B47" s="1">
         <v>14</v>
@@ -1375,7 +1372,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="1">
         <v>18</v>
@@ -1392,7 +1389,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1409,7 +1406,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B50" s="1">
         <v>6</v>
@@ -1426,7 +1423,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B51" s="1">
         <v>14</v>
@@ -1443,7 +1440,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B52" s="1">
         <v>18</v>
@@ -1460,7 +1457,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -1477,7 +1474,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B54" s="9">
         <v>6</v>
@@ -1492,7 +1489,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B55" s="9">
         <v>14</v>
@@ -1507,7 +1504,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B56" s="9">
         <v>18</v>
@@ -1522,7 +1519,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57" s="9">
         <v>0</v>
@@ -1537,7 +1534,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B58" s="10">
         <v>6</v>
@@ -1552,7 +1549,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B59" s="10">
         <v>9</v>
@@ -1567,7 +1564,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B60" s="10">
         <v>12</v>
@@ -1582,7 +1579,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B61" s="10">
         <v>15</v>
@@ -1597,7 +1594,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B62" s="10">
         <v>18</v>
@@ -1612,7 +1609,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B63" s="10">
         <v>21</v>
@@ -1627,7 +1624,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B64" s="10">
         <v>23</v>
@@ -1642,7 +1639,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
@@ -1657,7 +1654,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -1668,7 +1665,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B67" s="1">
         <v>6</v>
@@ -1685,7 +1682,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B68" s="1">
         <v>14</v>
@@ -1702,7 +1699,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B69" s="1">
         <v>18</v>
@@ -1719,7 +1716,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -1743,14 +1740,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4436599-CC40-4B1F-BA68-C79DB18047E4}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,43 +1807,43 @@
         <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E191E4-A2D8-441B-8AD8-3523E2EF823B}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,7 +1891,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>6</v>
@@ -1906,7 +1905,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1">
         <v>9</v>
@@ -1920,7 +1919,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -1934,7 +1933,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
@@ -1948,7 +1947,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -1962,7 +1961,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1">
         <v>21</v>
@@ -1976,7 +1975,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1">
         <v>23</v>
@@ -1990,7 +1989,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -2004,7 +2003,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="7">
         <v>1</v>
@@ -2018,7 +2017,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
Se implementó un print para registrar cuando no se encuentra la SEDE y la HORA ..
</commit_message>
<xml_diff>
--- a/data/tarifas_GFM.xlsx
+++ b/data/tarifas_GFM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\gfm\streamlit-demo\prod\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3F3797-A597-4089-A8CE-B6E381B29460}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3B5B0D-37CA-43CE-A74E-FED551AC96C3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" activeTab="1" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="34">
   <si>
     <t>PLAZA</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>158-TAMPICOCANAL1</t>
-  </si>
-  <si>
-    <t>TAMPICO</t>
   </si>
   <si>
     <t>160-SLPCANAL1</t>
@@ -930,7 +927,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>6</v>
@@ -947,7 +944,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>14</v>
@@ -964,7 +961,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
         <v>18</v>
@@ -981,7 +978,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -998,7 +995,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1">
         <v>6</v>
@@ -1015,7 +1012,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
         <v>14</v>
@@ -1032,7 +1029,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>18</v>
@@ -1049,7 +1046,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1134,7 +1131,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="1">
         <v>6</v>
@@ -1151,7 +1148,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1">
         <v>14</v>
@@ -1168,7 +1165,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="1">
         <v>18</v>
@@ -1185,7 +1182,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -1270,7 +1267,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="1">
         <v>6</v>
@@ -1287,7 +1284,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="1">
         <v>14</v>
@@ -1304,7 +1301,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="1">
         <v>18</v>
@@ -1321,7 +1318,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -1338,7 +1335,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B46" s="1">
         <v>6</v>
@@ -1355,7 +1352,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B47" s="1">
         <v>14</v>
@@ -1372,7 +1369,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="1">
         <v>18</v>
@@ -1389,7 +1386,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1406,7 +1403,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B50" s="1">
         <v>6</v>
@@ -1423,7 +1420,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B51" s="1">
         <v>14</v>
@@ -1440,7 +1437,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B52" s="1">
         <v>18</v>
@@ -1457,7 +1454,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -1474,7 +1471,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="9">
         <v>6</v>
@@ -1489,7 +1486,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B55" s="9">
         <v>14</v>
@@ -1504,7 +1501,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B56" s="9">
         <v>18</v>
@@ -1519,7 +1516,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B57" s="9">
         <v>0</v>
@@ -1534,7 +1531,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B58" s="10">
         <v>6</v>
@@ -1549,7 +1546,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B59" s="10">
         <v>9</v>
@@ -1564,7 +1561,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60" s="10">
         <v>12</v>
@@ -1579,7 +1576,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B61" s="10">
         <v>15</v>
@@ -1594,7 +1591,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B62" s="10">
         <v>18</v>
@@ -1609,7 +1606,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B63" s="10">
         <v>21</v>
@@ -1624,7 +1621,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B64" s="10">
         <v>23</v>
@@ -1639,7 +1636,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
@@ -1654,7 +1651,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -1665,7 +1662,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B67" s="1">
         <v>6</v>
@@ -1682,7 +1679,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B68" s="1">
         <v>14</v>
@@ -1699,7 +1696,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B69" s="1">
         <v>18</v>
@@ -1716,7 +1713,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -1741,7 +1738,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,7 +1804,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1827,23 +1824,23 @@
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1891,7 +1888,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1">
         <v>6</v>
@@ -1905,7 +1902,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1">
         <v>9</v>
@@ -1919,7 +1916,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -1933,7 +1930,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
@@ -1947,7 +1944,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -1961,7 +1958,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1">
         <v>21</v>
@@ -1975,7 +1972,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1">
         <v>23</v>
@@ -1989,7 +1986,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -2003,7 +2000,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="7">
         <v>1</v>
@@ -2017,7 +2014,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
Se implementó una primer optimización del algoritmo de clasificación ..
</commit_message>
<xml_diff>
--- a/data/tarifas_GFM.xlsx
+++ b/data/tarifas_GFM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\gfm\streamlit-demo\prod\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3B5B0D-37CA-43CE-A74E-FED551AC96C3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4049D7-A0DA-4B42-BDB7-8B24C325DBDF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" activeTab="1" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" xr2:uid="{00946C30-E23C-4134-908F-29F80C46C3A3}"/>
   </bookViews>
   <sheets>
     <sheet name="PLAZAS_TARIFAS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="33">
   <si>
     <t>PLAZA</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>GUADALAJARA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TORREON </t>
   </si>
   <si>
     <t>MATAMOROS</t>
@@ -557,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434E9FDD-879A-4363-B04D-C869C9708562}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,7 +1332,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B46" s="1">
         <v>6</v>
@@ -1352,7 +1349,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B47" s="1">
         <v>14</v>
@@ -1369,7 +1366,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B48" s="1">
         <v>18</v>
@@ -1386,7 +1383,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1403,7 +1400,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B50" s="1">
         <v>6</v>
@@ -1420,7 +1417,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B51" s="1">
         <v>14</v>
@@ -1437,7 +1434,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B52" s="1">
         <v>18</v>
@@ -1454,7 +1451,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -1471,7 +1468,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B54" s="9">
         <v>6</v>
@@ -1486,7 +1483,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B55" s="9">
         <v>14</v>
@@ -1501,7 +1498,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B56" s="9">
         <v>18</v>
@@ -1516,7 +1513,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57" s="9">
         <v>0</v>
@@ -1627,7 +1624,7 @@
         <v>23</v>
       </c>
       <c r="C64" s="10">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D64" s="10">
         <v>53901.65</v>
@@ -1737,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4436599-CC40-4B1F-BA68-C79DB18047E4}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1801,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1824,7 +1821,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,7 +1885,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1">
         <v>6</v>
@@ -1902,7 +1899,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1">
         <v>9</v>
@@ -1916,7 +1913,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -1930,7 +1927,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
@@ -1944,7 +1941,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>18</v>
@@ -1958,7 +1955,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1">
         <v>21</v>
@@ -1972,7 +1969,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
         <v>23</v>
@@ -1986,7 +1983,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -2000,7 +1997,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7">
         <v>1</v>
@@ -2014,7 +2011,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>

</xml_diff>